<commit_message>
Selecting all checklist fix
</commit_message>
<xml_diff>
--- a/src/test/resources/ReadGradeData.xlsx
+++ b/src/test/resources/ReadGradeData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="69">
   <si>
     <t>category_name</t>
   </si>
@@ -338,7 +338,7 @@
     <xf numFmtId="9" fontId="1" fillId="4" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -356,6 +356,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -709,7 +711,7 @@
       <c r="F2" s="11">
         <v>0.2</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="28" t="s">
         <v>55</v>
       </c>
     </row>
@@ -732,7 +734,7 @@
       <c r="F3" s="11">
         <v>0.19</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="29" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Committing the changes done in the framework.
</commit_message>
<xml_diff>
--- a/src/test/resources/ReadGradeData.xlsx
+++ b/src/test/resources/ReadGradeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaur\IdeaProjects\master_framework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shauryasmac/IdeaProjects/master_framework/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64756914-4181-40A7-A068-1736A176BDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F72CC4-3CCB-5945-98F1-EAE12346ACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="69">
   <si>
     <t>category_name</t>
   </si>
@@ -338,7 +338,7 @@
     <xf numFmtId="9" fontId="1" fillId="4" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -355,31 +355,13 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{1ACA6766-7DFF-4D36-BAB2-0D54792DCFA0}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{81D2685F-24FD-4B41-AE1E-7DFAC30B68BA}"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
     <cellStyle name="Per cent 2" xfId="3" xr:uid="{8A660E4F-918E-413D-92A5-8594959C692C}"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,19 +639,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="7.6640625"/>
-    <col min="6" max="6" customWidth="true" width="8.5546875"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -692,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>60</v>
       </c>
@@ -711,30 +693,7 @@
       <c r="F2" s="11">
         <v>0.2</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0.63749999999999996</v>
-      </c>
-      <c r="F3" s="11">
-        <v>0.19</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="G2" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -752,12 +711,12 @@
       <selection activeCell="A48" sqref="A48:F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="38.33203125"/>
+    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -803,7 +762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -826,7 +785,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -849,7 +808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -872,7 +831,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -895,7 +854,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -918,7 +877,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -941,7 +900,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -964,7 +923,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -987,7 +946,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1010,7 +969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +992,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1056,7 +1015,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1079,7 +1038,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1061,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -1125,7 +1084,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1148,7 +1107,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1171,7 +1130,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1153,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1217,7 +1176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1240,7 +1199,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -1263,7 +1222,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +1245,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1268,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
@@ -1332,7 +1291,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -1355,7 +1314,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
@@ -1378,7 +1337,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -1401,7 +1360,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -1424,7 +1383,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
@@ -1447,7 +1406,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -1470,7 +1429,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
@@ -1493,7 +1452,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
@@ -1516,7 +1475,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
@@ -1539,7 +1498,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -1562,7 +1521,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -1585,7 +1544,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -1608,7 +1567,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
@@ -1631,7 +1590,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1654,7 +1613,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
@@ -1677,7 +1636,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
@@ -1700,7 +1659,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -1723,7 +1682,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -1746,7 +1705,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -1769,7 +1728,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -1792,7 +1751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -1815,7 +1774,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1838,7 +1797,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>60</v>
       </c>
@@ -1861,7 +1820,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>60</v>
       </c>
@@ -1884,7 +1843,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>60</v>
       </c>
@@ -1907,7 +1866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>60</v>
       </c>
@@ -1930,7 +1889,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>60</v>
       </c>
@@ -1953,7 +1912,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>60</v>
       </c>
@@ -1976,7 +1935,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>60</v>
       </c>
@@ -1999,7 +1958,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>60</v>
       </c>
@@ -2022,7 +1981,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>60</v>
       </c>
@@ -2045,7 +2004,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>60</v>
       </c>
@@ -2068,7 +2027,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>60</v>
       </c>
@@ -2091,7 +2050,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>60</v>
       </c>
@@ -2114,7 +2073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -2137,7 +2096,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>60</v>
       </c>

</xml_diff>